<commit_message>
Remove elevation and runoff from TOC model and re-run
</commit_message>
<xml_diff>
--- a/summaries/exceedance_summaries_mar_2023.xlsx
+++ b/summaries/exceedance_summaries_mar_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D479B08E-3BC7-4AFB-9034-BB73F2E634D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5748DCFB-CE86-4B24-BC8A-2ECB225A4527}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{3603B101-56A8-4E49-9E74-DD4909CD7F11}"/>
+    <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11422" xr2:uid="{3603B101-56A8-4E49-9E74-DD4909CD7F11}"/>
   </bookViews>
   <sheets>
     <sheet name="vegetation" sheetId="1" r:id="rId1"/>
@@ -99,7 +99,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,13 +115,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -136,9 +148,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B50734D-A978-4AA7-A9E8-D70664EAA28E}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C24:C25"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -506,7 +521,7 @@
         <v>17</v>
       </c>
       <c r="D2">
-        <v>134628</v>
+        <v>134864</v>
       </c>
       <c r="E2">
         <v>320585</v>
@@ -526,7 +541,7 @@
         <v>17</v>
       </c>
       <c r="D3">
-        <v>144868</v>
+        <v>144876</v>
       </c>
       <c r="E3">
         <v>320585</v>
@@ -546,7 +561,7 @@
         <v>17</v>
       </c>
       <c r="D4">
-        <v>115873</v>
+        <v>116078</v>
       </c>
       <c r="E4">
         <v>320585</v>
@@ -566,7 +581,7 @@
         <v>17</v>
       </c>
       <c r="D5">
-        <v>108753</v>
+        <v>109212</v>
       </c>
       <c r="E5">
         <v>320585</v>
@@ -586,7 +601,7 @@
         <v>17</v>
       </c>
       <c r="D6">
-        <v>111974</v>
+        <v>112436</v>
       </c>
       <c r="E6">
         <v>320585</v>
@@ -606,13 +621,13 @@
         <v>17</v>
       </c>
       <c r="D7">
-        <v>116356</v>
+        <v>117009</v>
       </c>
       <c r="E7">
         <v>320391</v>
       </c>
       <c r="F7">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -626,7 +641,7 @@
         <v>17</v>
       </c>
       <c r="D8">
-        <v>115058</v>
+        <v>115739</v>
       </c>
       <c r="E8">
         <v>320585</v>
@@ -646,7 +661,7 @@
         <v>17</v>
       </c>
       <c r="D9">
-        <v>118971</v>
+        <v>119201</v>
       </c>
       <c r="E9">
         <v>320585</v>
@@ -666,7 +681,7 @@
         <v>17</v>
       </c>
       <c r="D10">
-        <v>115518</v>
+        <v>116794</v>
       </c>
       <c r="E10">
         <v>322183</v>
@@ -689,17 +704,44 @@
         <v>17</v>
       </c>
       <c r="D11">
-        <v>46303</v>
+        <v>46818</v>
       </c>
       <c r="E11">
         <v>322184</v>
       </c>
       <c r="F11">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G11" t="s">
         <v>19</v>
       </c>
+    </row>
+    <row r="31" spans="8:8" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="8:8" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="8:8" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="8:8" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="8:8" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="8:8" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="8:8" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="8:8" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="8:8" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="H39" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -711,7 +753,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G11"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -759,13 +801,13 @@
         <v>17</v>
       </c>
       <c r="D2">
-        <v>138492</v>
+        <v>134026</v>
       </c>
       <c r="E2">
         <v>320585</v>
       </c>
       <c r="F2">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -779,13 +821,13 @@
         <v>17</v>
       </c>
       <c r="D3">
-        <v>136634</v>
+        <v>133585</v>
       </c>
       <c r="E3">
         <v>320585</v>
       </c>
       <c r="F3">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
@@ -799,13 +841,13 @@
         <v>17</v>
       </c>
       <c r="D4">
-        <v>116361</v>
+        <v>111469</v>
       </c>
       <c r="E4">
         <v>320585</v>
       </c>
       <c r="F4">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
@@ -819,13 +861,13 @@
         <v>17</v>
       </c>
       <c r="D5">
-        <v>98049</v>
+        <v>92401</v>
       </c>
       <c r="E5">
         <v>320585</v>
       </c>
       <c r="F5">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
@@ -839,13 +881,13 @@
         <v>17</v>
       </c>
       <c r="D6">
-        <v>83120</v>
+        <v>78295</v>
       </c>
       <c r="E6">
         <v>320585</v>
       </c>
       <c r="F6">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
@@ -859,13 +901,13 @@
         <v>17</v>
       </c>
       <c r="D7">
-        <v>80434</v>
+        <v>75307</v>
       </c>
       <c r="E7">
         <v>320391</v>
       </c>
       <c r="F7">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -879,13 +921,13 @@
         <v>17</v>
       </c>
       <c r="D8">
-        <v>73796</v>
+        <v>68624</v>
       </c>
       <c r="E8">
         <v>320585</v>
       </c>
       <c r="F8">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
@@ -899,13 +941,13 @@
         <v>17</v>
       </c>
       <c r="D9">
-        <v>72601</v>
+        <v>67681</v>
       </c>
       <c r="E9">
         <v>320585</v>
       </c>
       <c r="F9">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
@@ -919,13 +961,13 @@
         <v>17</v>
       </c>
       <c r="D10">
-        <v>64966</v>
+        <v>61401</v>
       </c>
       <c r="E10">
         <v>322183</v>
       </c>
       <c r="F10">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G10" t="s">
         <v>18</v>
@@ -942,13 +984,13 @@
         <v>17</v>
       </c>
       <c r="D11">
-        <v>39787</v>
+        <v>35984</v>
       </c>
       <c r="E11">
         <v>322184</v>
       </c>
       <c r="F11">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G11" t="s">
         <v>19</v>
@@ -964,7 +1006,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1012,13 +1054,13 @@
         <v>17</v>
       </c>
       <c r="D2">
-        <v>104373</v>
+        <v>96872</v>
       </c>
       <c r="E2">
         <v>320585</v>
       </c>
       <c r="F2">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -1032,13 +1074,13 @@
         <v>17</v>
       </c>
       <c r="D3">
-        <v>103419</v>
+        <v>99274</v>
       </c>
       <c r="E3">
         <v>320585</v>
       </c>
       <c r="F3">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
@@ -1052,13 +1094,13 @@
         <v>17</v>
       </c>
       <c r="D4">
-        <v>87074</v>
+        <v>82805</v>
       </c>
       <c r="E4">
         <v>320585</v>
       </c>
       <c r="F4">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
@@ -1072,13 +1114,13 @@
         <v>17</v>
       </c>
       <c r="D5">
-        <v>65378</v>
+        <v>60258</v>
       </c>
       <c r="E5">
         <v>320585</v>
       </c>
       <c r="F5">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
@@ -1092,13 +1134,13 @@
         <v>17</v>
       </c>
       <c r="D6">
-        <v>50714</v>
+        <v>45762</v>
       </c>
       <c r="E6">
         <v>320585</v>
       </c>
       <c r="F6">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
@@ -1112,13 +1154,13 @@
         <v>17</v>
       </c>
       <c r="D7">
-        <v>41700</v>
+        <v>37780</v>
       </c>
       <c r="E7">
         <v>320391</v>
       </c>
       <c r="F7">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -1132,13 +1174,13 @@
         <v>17</v>
       </c>
       <c r="D8">
-        <v>34257</v>
+        <v>29194</v>
       </c>
       <c r="E8">
         <v>320585</v>
       </c>
       <c r="F8">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
@@ -1152,13 +1194,13 @@
         <v>17</v>
       </c>
       <c r="D9">
-        <v>30175</v>
+        <v>24695</v>
       </c>
       <c r="E9">
         <v>320585</v>
       </c>
       <c r="F9">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
@@ -1172,13 +1214,13 @@
         <v>17</v>
       </c>
       <c r="D10">
-        <v>24723</v>
+        <v>21121</v>
       </c>
       <c r="E10">
         <v>322183</v>
       </c>
       <c r="F10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G10" t="s">
         <v>18</v>
@@ -1195,13 +1237,13 @@
         <v>17</v>
       </c>
       <c r="D11">
-        <v>23634</v>
+        <v>20306</v>
       </c>
       <c r="E11">
         <v>322184</v>
       </c>
       <c r="F11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
16-bit => 32-bit to avoid overflow
</commit_message>
<xml_diff>
--- a/summaries/exceedance_summaries_mar_2023.xlsx
+++ b/summaries/exceedance_summaries_mar_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF87126-0D66-4F51-A42D-66C6F0200077}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A0BF80-20CC-4227-807A-56B919B1F85B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{3603B101-56A8-4E49-9E74-DD4909CD7F11}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{3603B101-56A8-4E49-9E74-DD4909CD7F11}"/>
   </bookViews>
   <sheets>
     <sheet name="vegetation" sheetId="1" r:id="rId1"/>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B50734D-A978-4AA7-A9E8-D70664EAA28E}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1259,8 +1259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5837D15-4DB9-466A-A2C2-EA69DFE6AD6B}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1301,7 +1301,7 @@
         <v>16</v>
       </c>
       <c r="C2">
-        <v>1890</v>
+        <v>1379</v>
       </c>
       <c r="D2">
         <v>320585</v>
@@ -1319,7 +1319,7 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>2359</v>
+        <v>1848</v>
       </c>
       <c r="D3">
         <v>320585</v>
@@ -1337,7 +1337,7 @@
         <v>16</v>
       </c>
       <c r="C4">
-        <v>1307</v>
+        <v>796</v>
       </c>
       <c r="D4">
         <v>320585</v>
@@ -1355,7 +1355,7 @@
         <v>16</v>
       </c>
       <c r="C5">
-        <v>710</v>
+        <v>199</v>
       </c>
       <c r="D5">
         <v>320585</v>
@@ -1373,7 +1373,7 @@
         <v>16</v>
       </c>
       <c r="C6">
-        <v>511</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>320585</v>
@@ -1391,7 +1391,7 @@
         <v>16</v>
       </c>
       <c r="C7">
-        <v>511</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>320391</v>
@@ -1409,7 +1409,7 @@
         <v>16</v>
       </c>
       <c r="C8">
-        <v>511</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>320585</v>
@@ -1427,7 +1427,7 @@
         <v>16</v>
       </c>
       <c r="C9">
-        <v>511</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>320585</v>
@@ -1445,7 +1445,7 @@
         <v>16</v>
       </c>
       <c r="C10">
-        <v>511</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <v>322183</v>
@@ -1466,7 +1466,7 @@
         <v>17</v>
       </c>
       <c r="C11">
-        <v>510</v>
+        <v>0</v>
       </c>
       <c r="D11">
         <v>322184</v>

</xml_diff>